<commit_message>
olx automaiton is completed almost 95%
</commit_message>
<xml_diff>
--- a/Automation/olx/DataFile/Testdata.xlsx
+++ b/Automation/olx/DataFile/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtpl/Automation/olx/DataFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C6FA37-C641-D54D-B606-C0EF275F7F40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF3B31E-17E1-D54E-840B-5AD8EC4EDDC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -46,35 +46,53 @@
     <t>lname2</t>
   </si>
   <si>
-    <t>BranchName</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Madhapur</t>
-  </si>
-  <si>
-    <t>david</t>
-  </si>
-  <si>
-    <t>Kukatpally</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Ameerpet</t>
-  </si>
-  <si>
-    <t>Richards</t>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Choose Location</t>
+  </si>
+  <si>
+    <t>Contact Person</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>77079154354</t>
+  </si>
+  <si>
+    <t>KNF8KBMK</t>
+  </si>
+  <si>
+    <t>792267SM</t>
+  </si>
+  <si>
+    <t>AKPEPT37</t>
+  </si>
+  <si>
+    <t>77767517099</t>
+  </si>
+  <si>
+    <t>77767517078</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +107,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,48 +419,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>